<commit_message>
started working on mixture vapor pressure
</commit_message>
<xml_diff>
--- a/Table 7-1-6 Paint solar absortance.xlsx
+++ b/Table 7-1-6 Paint solar absortance.xlsx
@@ -1,21 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4505"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="124226"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\EricKim\Documents\AP42\AP42-Emissions-py\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{357795E4-A7C2-41E9-BE24-405F8140AE3D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="18240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="1" r:id="rId1"/>
     <sheet name="Descriptions" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="124519" fullCalcOnLoad="1"/>
+  <calcPr calcId="124519"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="68" uniqueCount="55">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="26">
   <si>
     <t>surface color</t>
   </si>
@@ -66,93 +72,6 @@
   </si>
   <si>
     <t>unpainted aluminum</t>
-  </si>
-  <si>
-    <t>0.17</t>
-  </si>
-  <si>
-    <t>0.39</t>
-  </si>
-  <si>
-    <t>0.60</t>
-  </si>
-  <si>
-    <t>0.35</t>
-  </si>
-  <si>
-    <t>0.97</t>
-  </si>
-  <si>
-    <t>0.58</t>
-  </si>
-  <si>
-    <t>0.54</t>
-  </si>
-  <si>
-    <t>0.68</t>
-  </si>
-  <si>
-    <t>0.89</t>
-  </si>
-  <si>
-    <t>0.38</t>
-  </si>
-  <si>
-    <t>0.43</t>
-  </si>
-  <si>
-    <t>0.10</t>
-  </si>
-  <si>
-    <t>0.25</t>
-  </si>
-  <si>
-    <t>0.44</t>
-  </si>
-  <si>
-    <t>0.64</t>
-  </si>
-  <si>
-    <t>0.42</t>
-  </si>
-  <si>
-    <t>0.62</t>
-  </si>
-  <si>
-    <t>0.71</t>
-  </si>
-  <si>
-    <t>0.90</t>
-  </si>
-  <si>
-    <t>0.49</t>
-  </si>
-  <si>
-    <t>0.12</t>
-  </si>
-  <si>
-    <t>0.34</t>
-  </si>
-  <si>
-    <t>0.67</t>
-  </si>
-  <si>
-    <t>0.63</t>
-  </si>
-  <si>
-    <t>0.74</t>
-  </si>
-  <si>
-    <t>0.91</t>
-  </si>
-  <si>
-    <t>0.50</t>
-  </si>
-  <si>
-    <t>0.55</t>
-  </si>
-  <si>
-    <t>0.15</t>
   </si>
   <si>
     <t>Symbol</t>
@@ -185,8 +104,8 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -238,24 +157,33 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme 2007 - 2010">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2007 - 2010">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -293,7 +221,7 @@
         <a:srgbClr val="800080"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2007 - 2010">
       <a:majorFont>
         <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
@@ -327,6 +255,7 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
         <a:latin typeface="Calibri"/>
@@ -361,9 +290,10 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2007 - 2010">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -536,14 +466,19 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="19.85546875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -557,186 +492,186 @@
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="B2" t="s">
-        <v>17</v>
-      </c>
-      <c r="C2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D2" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4">
+      <c r="B2" s="2">
+        <v>0.17</v>
+      </c>
+      <c r="C2" s="2">
+        <v>0.25</v>
+      </c>
+      <c r="D2" s="2">
+        <v>0.34</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C3" t="s">
-        <v>30</v>
-      </c>
-      <c r="D3" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4">
+      <c r="B3" s="2">
+        <v>0.39</v>
+      </c>
+      <c r="C3" s="2">
+        <v>0.44</v>
+      </c>
+      <c r="D3" s="2">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>6</v>
       </c>
-      <c r="B4" t="s">
-        <v>19</v>
-      </c>
-      <c r="C4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D4" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4">
+      <c r="B4" s="2">
+        <v>0.6</v>
+      </c>
+      <c r="C4" s="2">
+        <v>0.64</v>
+      </c>
+      <c r="D4" s="2">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>7</v>
       </c>
-      <c r="B5" t="s">
-        <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D5" t="s">
-        <v>36</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4">
+      <c r="B5" s="2">
+        <v>0.35</v>
+      </c>
+      <c r="C5" s="2">
+        <v>0.42</v>
+      </c>
+      <c r="D5" s="2">
+        <v>0.49</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>8</v>
       </c>
-      <c r="B6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C6" t="s">
-        <v>21</v>
-      </c>
-      <c r="D6" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
+      <c r="B6" s="2">
+        <v>0.97</v>
+      </c>
+      <c r="C6" s="2">
+        <v>0.97</v>
+      </c>
+      <c r="D6" s="2">
+        <v>0.97</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>9</v>
       </c>
-      <c r="B7" t="s">
-        <v>22</v>
-      </c>
-      <c r="C7" t="s">
-        <v>33</v>
-      </c>
-      <c r="D7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
+      <c r="B7" s="2">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="C7" s="2">
+        <v>0.62</v>
+      </c>
+      <c r="D7" s="2">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>10</v>
       </c>
-      <c r="B8" t="s">
-        <v>23</v>
-      </c>
-      <c r="C8" t="s">
-        <v>22</v>
-      </c>
-      <c r="D8" t="s">
-        <v>40</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
+      <c r="B8" s="2">
+        <v>0.54</v>
+      </c>
+      <c r="C8" s="2">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="D8" s="2">
+        <v>0.63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>11</v>
       </c>
-      <c r="B9" t="s">
-        <v>24</v>
-      </c>
-      <c r="C9" t="s">
-        <v>34</v>
-      </c>
-      <c r="D9" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
+      <c r="B9" s="2">
+        <v>0.68</v>
+      </c>
+      <c r="C9" s="2">
+        <v>0.71</v>
+      </c>
+      <c r="D9" s="2">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>12</v>
       </c>
-      <c r="B10" t="s">
-        <v>25</v>
-      </c>
-      <c r="C10" t="s">
-        <v>35</v>
-      </c>
-      <c r="D10" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4">
+      <c r="B10" s="2">
+        <v>0.89</v>
+      </c>
+      <c r="C10" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="D10" s="2">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>13</v>
       </c>
-      <c r="B11" t="s">
-        <v>25</v>
-      </c>
-      <c r="C11" t="s">
-        <v>35</v>
-      </c>
-      <c r="D11" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4">
+      <c r="B11" s="2">
+        <v>0.89</v>
+      </c>
+      <c r="C11" s="2">
+        <v>0.9</v>
+      </c>
+      <c r="D11" s="2">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>14</v>
       </c>
-      <c r="B12" t="s">
-        <v>26</v>
-      </c>
-      <c r="C12" t="s">
-        <v>30</v>
-      </c>
-      <c r="D12" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4">
+      <c r="B12" s="2">
+        <v>0.38</v>
+      </c>
+      <c r="C12" s="2">
+        <v>0.44</v>
+      </c>
+      <c r="D12" s="2">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>15</v>
       </c>
-      <c r="B13" t="s">
-        <v>27</v>
-      </c>
-      <c r="C13" t="s">
-        <v>36</v>
-      </c>
-      <c r="D13" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4">
+      <c r="B13" s="2">
+        <v>0.43</v>
+      </c>
+      <c r="C13" s="2">
+        <v>0.49</v>
+      </c>
+      <c r="D13" s="2">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>16</v>
       </c>
-      <c r="B14" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" t="s">
-        <v>37</v>
-      </c>
-      <c r="D14" t="s">
-        <v>45</v>
+      <c r="B14" s="2">
+        <v>0.1</v>
+      </c>
+      <c r="C14" s="2">
+        <v>0.12</v>
+      </c>
+      <c r="D14" s="2">
+        <v>0.15</v>
       </c>
     </row>
   </sheetData>
@@ -745,59 +680,59 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>46</v>
+        <v>17</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>47</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>48</v>
+        <v>19</v>
       </c>
       <c r="B5" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>49</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>54</v>
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>